<commit_message>
Modification du modèle + ajout fichiers
</commit_message>
<xml_diff>
--- a/modele/data/niveau_de_vie.xlsx
+++ b/modele/data/niveau_de_vie.xlsx
@@ -22,15 +22,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="399" uniqueCount="388">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="399" uniqueCount="389">
   <si>
     <t xml:space="preserve">libelle_commune</t>
   </si>
   <si>
-    <t xml:space="preserve">Nb de ménages fiscaux 2021</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Médiane du niveau de vie 2021</t>
+    <t xml:space="preserve">Nb_de_ménages_fiscaux</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Médiane_du_niveau_de_vie</t>
   </si>
   <si>
     <t xml:space="preserve">annee</t>
@@ -1174,6 +1174,9 @@
   </si>
   <si>
     <t xml:space="preserve">https://statistiques-locales.insee.fr/index.php?view=map1&amp;indics=filosofi.nbmenfisc&amp;serie=2021&amp;lang=fr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Médiane du niveau de vie 2021</t>
   </si>
   <si>
     <t xml:space="preserve">Unité</t>
@@ -1328,7 +1331,7 @@
   <dimension ref="A1:D1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.50390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6917,7 +6920,7 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>2</v>
+        <v>383</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6932,12 +6935,12 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="4" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="5" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6947,7 +6950,7 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="5" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6967,7 +6970,7 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="5" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6987,7 +6990,7 @@
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="6" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
     </row>
   </sheetData>

</xml_diff>